<commit_message>
Extended dataset object structure
* Additional members added 12/27/2019 by DPC
* Make it easier to correlate the NL and LL values with those in the Excel file and catch data entry errors in `DfReadDataFile()`
   + design = design,
   +  normalCases = normalCases,
   +  abnormalCases = abnormalCases,
   +  truthTableStr = truthTableStr
* Need to update all datasets and check all occurences where `DfReadDataFile()` is used
ran R CMD check with file size note 12.6 Mb
</commit_message>
<xml_diff>
--- a/inst/extdata/toyFiles/FROC/frocCr2BlankRows.xlsx
+++ b/inst/extdata/toyFiles/FROC/frocCr2BlankRows.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dev/GitHub/RJafroc/inst/extdata/toyFiles/FROC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CA5CE72-78AE-B54D-BE74-41CC28B904B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E69F2765-E11A-7B4F-961E-BB6120D5B4F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="760" windowWidth="10000" windowHeight="10860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13720" yWindow="1140" windowWidth="10440" windowHeight="10080" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TP" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="15">
   <si>
     <t>CaseID</t>
   </si>
@@ -75,18 +75,6 @@
   </si>
   <si>
     <t>FROC</t>
-  </si>
-  <si>
-    <t>0.1</t>
-  </si>
-  <si>
-    <t>0.9</t>
-  </si>
-  <si>
-    <t>0.3</t>
-  </si>
-  <si>
-    <t>0.7</t>
   </si>
   <si>
     <t>crossed</t>
@@ -189,12 +177,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -584,18 +575,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="A1:G1048576"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="5" width="8.83203125" style="1"/>
+    <col min="8" max="8" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -611,12 +603,12 @@
       <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1">
+      <c r="M1">
         <f ca="1">RAND()-0.5</f>
-        <v>0.27510073386161948</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>-0.10064690581480384</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -632,16 +624,16 @@
       <c r="E2" s="1">
         <v>5.28</v>
       </c>
-      <c r="G2">
-        <f t="shared" ref="G2:G9" ca="1" si="0">ROUND(0.5*(RAND()-0.5)+E2, 2)</f>
-        <v>5.09</v>
-      </c>
       <c r="J2">
-        <f t="shared" ref="J2:J34" ca="1" si="1">RAND()-0.5</f>
-        <v>8.2214842813328803E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+        <f t="shared" ref="J2:J5" ca="1" si="0">ROUND(0.5*(RAND()-0.5)+E2, 2)</f>
+        <v>5.38</v>
+      </c>
+      <c r="M2">
+        <f t="shared" ref="M2:M13" ca="1" si="1">RAND()-0.5</f>
+        <v>0.14177236812423755</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -657,16 +649,16 @@
       <c r="E3" s="1">
         <v>4.6500000000000004</v>
       </c>
-      <c r="G3">
+      <c r="J3">
         <f t="shared" ca="1" si="0"/>
-        <v>4.8499999999999996</v>
-      </c>
-      <c r="J3">
+        <v>4.58</v>
+      </c>
+      <c r="M3">
         <f t="shared" ca="1" si="1"/>
-        <v>0.48610087079853515</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>9.8487006428479851E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -682,16 +674,16 @@
       <c r="E4" s="1">
         <v>3.01</v>
       </c>
-      <c r="G4">
+      <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>2.98</v>
-      </c>
-      <c r="J4">
+        <v>3.04</v>
+      </c>
+      <c r="M4">
         <f t="shared" ca="1" si="1"/>
-        <v>0.10605301805270095</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>-0.35811926024486351</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -707,16 +699,16 @@
       <c r="E5" s="1">
         <v>5.98</v>
       </c>
-      <c r="G5">
+      <c r="J5">
         <f t="shared" ca="1" si="0"/>
-        <v>5.95</v>
-      </c>
-      <c r="J5">
+        <v>5.87</v>
+      </c>
+      <c r="M5">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.3586832719813966</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>6.9581376979028553E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -732,12 +724,16 @@
       <c r="E6" s="1">
         <v>5</v>
       </c>
-      <c r="G6">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <f t="shared" ref="J6:J11" ca="1" si="2">ROUND(0.5*(RAND()-0.5)+E6, 2)</f>
+        <v>4.99</v>
+      </c>
+      <c r="M6">
+        <f t="shared" ca="1" si="1"/>
+        <v>-0.40749958051559609</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -753,16 +749,16 @@
       <c r="E7" s="1">
         <v>5.25</v>
       </c>
-      <c r="G7">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.42</v>
-      </c>
       <c r="J7">
+        <f t="shared" ca="1" si="2"/>
+        <v>5.05</v>
+      </c>
+      <c r="M7">
         <f t="shared" ca="1" si="1"/>
-        <v>0.44269830245419683</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0.19071767820466956</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -778,16 +774,16 @@
       <c r="E8" s="1">
         <v>4.26</v>
       </c>
-      <c r="G8">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.41</v>
-      </c>
       <c r="J8">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="M8">
         <f t="shared" ca="1" si="1"/>
-        <v>0.42210094996022163</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0.38373411632102061</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -803,16 +799,16 @@
       <c r="E9" s="1">
         <v>5.14</v>
       </c>
-      <c r="G9">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.01</v>
-      </c>
       <c r="J9">
+        <f t="shared" ca="1" si="2"/>
+        <v>4.91</v>
+      </c>
+      <c r="M9">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.41043653512839606</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0.10033668333807677</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -828,16 +824,16 @@
       <c r="E10" s="1">
         <v>3.31</v>
       </c>
-      <c r="G10">
-        <f t="shared" ref="G10:G32" ca="1" si="2">ROUND(0.5*(RAND()-0.5)+E10, 2)</f>
-        <v>3.19</v>
-      </c>
       <c r="J10">
+        <f t="shared" ca="1" si="2"/>
+        <v>3.28</v>
+      </c>
+      <c r="M10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.46542335162849902</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0.47743239795038561</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -853,16 +849,16 @@
       <c r="E11" s="1">
         <v>4.92</v>
       </c>
-      <c r="G11">
+      <c r="J11">
         <f t="shared" ca="1" si="2"/>
-        <v>4.82</v>
-      </c>
-      <c r="J11">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="M11">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.11655801129728893</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+        <v>-2.045598571700169E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
@@ -878,16 +874,12 @@
       <c r="E12" s="1">
         <v>5.1100000000000003</v>
       </c>
-      <c r="G12">
-        <f t="shared" ca="1" si="2"/>
-        <v>5.28</v>
-      </c>
-      <c r="J12">
+      <c r="M12">
         <f t="shared" ca="1" si="1"/>
-        <v>0.40324585773390786</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+        <v>2.6435032903818101E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
@@ -903,16 +895,12 @@
       <c r="E13" s="1">
         <v>4.63</v>
       </c>
-      <c r="G13">
-        <f t="shared" ca="1" si="2"/>
-        <v>4.4400000000000004</v>
-      </c>
-      <c r="J13">
+      <c r="M13">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.34308979743896173</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+        <v>0.18699920422213456</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
@@ -928,16 +916,8 @@
       <c r="E14" s="1">
         <v>4.95</v>
       </c>
-      <c r="G14">
-        <f t="shared" ca="1" si="2"/>
-        <v>5.14</v>
-      </c>
-      <c r="J14">
-        <f t="shared" ca="1" si="1"/>
-        <v>2.3076093230665173E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
@@ -953,16 +933,12 @@
       <c r="E15" s="1">
         <v>5.3</v>
       </c>
-      <c r="G15">
-        <f t="shared" ca="1" si="2"/>
-        <v>5.0599999999999996</v>
-      </c>
-      <c r="J15">
-        <f t="shared" ca="1" si="1"/>
-        <v>-0.44774343601945932</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M15">
+        <f ca="1">AVERAGE(M1:M13)</f>
+        <v>6.2091116871145199E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -978,16 +954,8 @@
       <c r="E16" s="1">
         <v>4.66</v>
       </c>
-      <c r="G16">
-        <f t="shared" ca="1" si="2"/>
-        <v>4.53</v>
-      </c>
-      <c r="J16">
-        <f t="shared" ca="1" si="1"/>
-        <v>-2.7502700164898641E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
@@ -1003,16 +971,8 @@
       <c r="E17" s="1">
         <v>4.03</v>
       </c>
-      <c r="G17">
-        <f t="shared" ca="1" si="2"/>
-        <v>4.16</v>
-      </c>
-      <c r="J17">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.45526189240663018</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
@@ -1028,16 +988,8 @@
       <c r="E18" s="1">
         <v>5.22</v>
       </c>
-      <c r="G18">
-        <f t="shared" ca="1" si="2"/>
-        <v>5.21</v>
-      </c>
-      <c r="J18">
-        <f t="shared" ca="1" si="1"/>
-        <v>2.1177131969770668E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
@@ -1053,16 +1005,8 @@
       <c r="E19" s="1">
         <v>4.9400000000000004</v>
       </c>
-      <c r="G19">
-        <f t="shared" ca="1" si="2"/>
-        <v>5.0999999999999996</v>
-      </c>
-      <c r="J19">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.36521756589729715</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>8</v>
       </c>
@@ -1078,16 +1022,8 @@
       <c r="E20" s="1">
         <v>5.27</v>
       </c>
-      <c r="G20">
-        <f t="shared" ca="1" si="2"/>
-        <v>5.1100000000000003</v>
-      </c>
-      <c r="J20">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.1796158258057281</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>6</v>
       </c>
@@ -1103,16 +1039,8 @@
       <c r="E21" s="1">
         <v>5.2</v>
       </c>
-      <c r="G21">
-        <f t="shared" ca="1" si="2"/>
-        <v>5.44</v>
-      </c>
-      <c r="J21">
-        <f t="shared" ca="1" si="1"/>
-        <v>-0.11627879629947613</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>6</v>
       </c>
@@ -1128,16 +1056,8 @@
       <c r="E22" s="1">
         <v>3.27</v>
       </c>
-      <c r="G22">
-        <f t="shared" ca="1" si="2"/>
-        <v>3.34</v>
-      </c>
-      <c r="J22">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.13277857803646387</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>6</v>
       </c>
@@ -1153,16 +1073,8 @@
       <c r="E23" s="1">
         <v>4.6100000000000003</v>
       </c>
-      <c r="G23">
-        <f t="shared" ca="1" si="2"/>
-        <v>4.57</v>
-      </c>
-      <c r="J23">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.44452920754831593</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>6</v>
       </c>
@@ -1178,16 +1090,8 @@
       <c r="E24" s="1">
         <v>5.18</v>
       </c>
-      <c r="G24">
-        <f t="shared" ca="1" si="2"/>
-        <v>5.12</v>
-      </c>
-      <c r="J24">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.10948107177781441</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>6</v>
       </c>
@@ -1203,16 +1107,8 @@
       <c r="E25" s="1">
         <v>4.72</v>
       </c>
-      <c r="G25">
-        <f t="shared" ca="1" si="2"/>
-        <v>4.93</v>
-      </c>
-      <c r="J25">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.40528218165591678</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>7</v>
       </c>
@@ -1228,16 +1124,8 @@
       <c r="E26" s="1">
         <v>4.7699999999999996</v>
       </c>
-      <c r="G26">
-        <f t="shared" ca="1" si="2"/>
-        <v>4.74</v>
-      </c>
-      <c r="J26">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.39239693036479295</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>7</v>
       </c>
@@ -1253,16 +1141,8 @@
       <c r="E27" s="1">
         <v>3.19</v>
       </c>
-      <c r="G27">
-        <f t="shared" ca="1" si="2"/>
-        <v>3.42</v>
-      </c>
-      <c r="J27">
-        <f t="shared" ca="1" si="1"/>
-        <v>-2.1477799206644277E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>7</v>
       </c>
@@ -1278,16 +1158,8 @@
       <c r="E28" s="1">
         <v>5.2</v>
       </c>
-      <c r="G28">
-        <f t="shared" ca="1" si="2"/>
-        <v>5.27</v>
-      </c>
-      <c r="J28">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.44637741388461882</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>7</v>
       </c>
@@ -1303,16 +1175,8 @@
       <c r="E29" s="1">
         <v>5.39</v>
       </c>
-      <c r="G29">
-        <f t="shared" ca="1" si="2"/>
-        <v>5.17</v>
-      </c>
-      <c r="J29">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.13263344541784006</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>7</v>
       </c>
@@ -1328,16 +1192,8 @@
       <c r="E30" s="1">
         <v>5.01</v>
       </c>
-      <c r="G30">
-        <f t="shared" ca="1" si="2"/>
-        <v>5.16</v>
-      </c>
-      <c r="J30">
-        <f t="shared" ca="1" si="1"/>
-        <v>-5.9018811902553758E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -1353,16 +1209,8 @@
       <c r="E31" s="1">
         <v>4.87</v>
       </c>
-      <c r="G31">
-        <f t="shared" ca="1" si="2"/>
-        <v>4.78</v>
-      </c>
-      <c r="J31">
-        <f t="shared" ca="1" si="1"/>
-        <v>-1.0205022234472949E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -1377,40 +1225,11 @@
       </c>
       <c r="E32" s="1">
         <v>1.94</v>
-      </c>
-      <c r="G32">
-        <f t="shared" ca="1" si="2"/>
-        <v>2.19</v>
-      </c>
-      <c r="J32">
-        <f t="shared" ca="1" si="1"/>
-        <v>-0.16530293791363748</v>
-      </c>
-    </row>
-    <row r="33" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J33">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.49291724882677257</v>
-      </c>
-    </row>
-    <row r="34" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J34">
-        <f t="shared" ca="1" si="1"/>
-        <v>-8.8573995796708216E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="10:10" x14ac:dyDescent="0.2">
-      <c r="J36">
-        <f ca="1">AVERAGE(J1:J34)</f>
-        <v>0.12481246662853766</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <ignoredErrors>
-    <ignoredError sqref="A7:B32 A2:B5" numberStoredAsText="1"/>
-  </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1421,18 +1240,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="A1:F1048576"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="4" width="8.83203125" style="1"/>
+    <col min="7" max="8" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1446,7 +1266,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1459,12 +1279,12 @@
       <c r="D2" s="1">
         <v>1.02</v>
       </c>
-      <c r="F2">
-        <f ca="1">ROUND(0.5*(RAND()-0.5)+D2, 2)</f>
-        <v>1.18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <f t="shared" ref="J2:J11" ca="1" si="0">ROUND(0.5*(RAND()-0.5)+D2, 2)</f>
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1477,12 +1297,12 @@
       <c r="D3" s="1">
         <v>2.17</v>
       </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F23" ca="1" si="0">ROUND(0.5*(RAND()-0.5)+D3, 2)</f>
-        <v>2.29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1495,12 +1315,12 @@
       <c r="D4" s="1">
         <v>2.2200000000000002</v>
       </c>
-      <c r="F4">
+      <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>2.25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>2.46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1513,12 +1333,12 @@
       <c r="D5" s="1">
         <v>1.9</v>
       </c>
-      <c r="F5">
+      <c r="J5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1.89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1531,66 +1351,62 @@
       <c r="D6" s="1">
         <v>2.21</v>
       </c>
-      <c r="F6">
+      <c r="J6">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.2599999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="J7">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2.21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="J9">
         <f t="shared" ca="1" si="0"/>
         <v>2.2200000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1">
-        <v>2</v>
-      </c>
-      <c r="D7" s="1">
-        <v>3.1</v>
-      </c>
-      <c r="F7">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="1">
-        <v>2</v>
-      </c>
-      <c r="D8" s="1">
-        <v>2.21</v>
-      </c>
-      <c r="F8">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="1">
-        <v>3</v>
-      </c>
-      <c r="D9" s="1">
-        <v>2.0699999999999998</v>
-      </c>
-      <c r="F9">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1603,12 +1419,12 @@
       <c r="D10" s="1">
         <v>2.14</v>
       </c>
-      <c r="F10">
+      <c r="J10">
         <f t="shared" ca="1" si="0"/>
-        <v>2.25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>2.33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -1621,12 +1437,12 @@
       <c r="D11" s="1">
         <v>1.98</v>
       </c>
-      <c r="F11">
+      <c r="J11">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1.91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -1639,12 +1455,8 @@
       <c r="D12" s="1">
         <v>1.95</v>
       </c>
-      <c r="F12">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
@@ -1657,12 +1469,8 @@
       <c r="D13" s="1">
         <v>2.89</v>
       </c>
-      <c r="F13">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.08</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -1675,12 +1483,8 @@
       <c r="D14" s="1">
         <v>2.89</v>
       </c>
-      <c r="F14">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -1688,17 +1492,13 @@
         <v>7</v>
       </c>
       <c r="C15" s="1">
-        <v>3</v>
+        <v>74</v>
       </c>
       <c r="D15" s="1">
         <v>0.84</v>
       </c>
-      <c r="F15">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
@@ -1706,17 +1506,13 @@
         <v>7</v>
       </c>
       <c r="C16" s="1">
-        <v>3</v>
+        <v>73</v>
       </c>
       <c r="D16" s="1">
         <v>1.85</v>
       </c>
-      <c r="F16">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.91</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -1729,12 +1525,8 @@
       <c r="D17" s="1">
         <v>3.22</v>
       </c>
-      <c r="F17">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.03</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>7</v>
       </c>
@@ -1747,12 +1539,8 @@
       <c r="D18" s="1">
         <v>3.01</v>
       </c>
-      <c r="F18">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.01</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -1765,12 +1553,8 @@
       <c r="D19" s="1">
         <v>1.96</v>
       </c>
-      <c r="F19">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.86</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
@@ -1783,12 +1567,8 @@
       <c r="D20" s="1">
         <v>2.08</v>
       </c>
-      <c r="F20">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
@@ -1796,17 +1576,13 @@
         <v>7</v>
       </c>
       <c r="C21" s="1">
-        <v>1</v>
+        <v>71</v>
       </c>
       <c r="D21" s="1">
         <v>2.2400000000000002</v>
       </c>
-      <c r="F21">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>8</v>
       </c>
@@ -1814,17 +1590,13 @@
         <v>7</v>
       </c>
       <c r="C22" s="1">
-        <v>2</v>
+        <v>71</v>
       </c>
       <c r="D22" s="1">
         <v>4.01</v>
       </c>
-      <c r="F22">
-        <f t="shared" ca="1" si="0"/>
-        <v>4.05</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>8</v>
       </c>
@@ -1832,22 +1604,15 @@
         <v>7</v>
       </c>
       <c r="C23" s="1">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="D23" s="1">
         <v>1.86</v>
-      </c>
-      <c r="F23">
-        <f t="shared" ca="1" si="0"/>
-        <v>1.98</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <ignoredErrors>
-    <ignoredError sqref="A2:B23" numberStoredAsText="1"/>
-  </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1861,7 +1626,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="A6" sqref="A6:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1929,7 +1694,7 @@
         <v>11</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1957,8 +1722,8 @@
       <c r="B5" s="2">
         <v>1</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>16</v>
+      <c r="C5" s="3">
+        <v>0.3</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
@@ -1971,7 +1736,7 @@
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="C6" s="3"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6"/>
@@ -1979,7 +1744,7 @@
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="C7" s="3"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7"/>
@@ -1991,8 +1756,8 @@
       <c r="B8" s="2">
         <v>2</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>17</v>
+      <c r="C8" s="3">
+        <v>0.7</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
@@ -2081,8 +1846,8 @@
       <c r="B13" s="2">
         <v>1</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>14</v>
+      <c r="C13" s="3">
+        <v>0.1</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>10</v>
@@ -2096,11 +1861,11 @@
       <c r="A14" s="2">
         <v>73</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>15</v>
+      <c r="B14" s="3">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.9</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>10</v>

</xml_diff>